<commit_message>
Added SSD and RSD to CommonDesigns.xlsx
</commit_message>
<xml_diff>
--- a/CommonDesigns.xlsx
+++ b/CommonDesigns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jordi_Classes_234\DOE\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71DA807-EE60-4B02-A268-A563A353C246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4DBF89-49E5-4B54-9119-E64E5E881BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B1F4CC8-6E29-4DF5-9B9B-812FEB45778E}"/>
   </bookViews>
@@ -33,6 +33,16 @@
     <sheet name="L32" sheetId="14" r:id="rId18"/>
     <sheet name="L36" sheetId="21" r:id="rId19"/>
     <sheet name="L'36" sheetId="22" r:id="rId20"/>
+    <sheet name="YL8" sheetId="24" r:id="rId21"/>
+    <sheet name="CCCD_2F" sheetId="25" r:id="rId22"/>
+    <sheet name="CCCD_3F" sheetId="26" r:id="rId23"/>
+    <sheet name="CCCD_4F" sheetId="27" r:id="rId24"/>
+    <sheet name="BBD_3F" sheetId="28" r:id="rId25"/>
+    <sheet name="BBD_4F" sheetId="29" r:id="rId26"/>
+    <sheet name="DD_2F" sheetId="32" r:id="rId27"/>
+    <sheet name="DD_3F" sheetId="31" r:id="rId28"/>
+    <sheet name="DD_4F" sheetId="30" r:id="rId29"/>
+    <sheet name="DSD" sheetId="33" r:id="rId30"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="121">
   <si>
     <t>A</t>
   </si>
@@ -465,6 +475,189 @@
   <si>
     <t>L'36</t>
   </si>
+  <si>
+    <t>2-level supersaturated designs</t>
+  </si>
+  <si>
+    <t>X32</t>
+  </si>
+  <si>
+    <t>X33</t>
+  </si>
+  <si>
+    <t>X34</t>
+  </si>
+  <si>
+    <t>X35</t>
+  </si>
+  <si>
+    <r>
+      <t>Yamada, S., &amp; Lin, D. K. (1997). Supersaturated design including an orthogonal base. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Canadian Journal of Statistics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 25(2), 203-213.</t>
+    </r>
+  </si>
+  <si>
+    <t>YL8</t>
+  </si>
+  <si>
+    <t>Central composite designs</t>
+  </si>
+  <si>
+    <t>circumscribed</t>
+  </si>
+  <si>
+    <r>
+      <t>Box, G. E. P., &amp; Wilson, K. B. (1951). On the Experimental Attainment of Optimum Conditions.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Journal of the Royal Statistical Society: Series B (Methodological)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 13(1), 1-38.</t>
+    </r>
+  </si>
+  <si>
+    <t>Alpha values selected for rotatability.</t>
+  </si>
+  <si>
+    <t>CCCD_2F</t>
+  </si>
+  <si>
+    <t>CCCD_3F</t>
+  </si>
+  <si>
+    <t>CCCD_4F</t>
+  </si>
+  <si>
+    <t>Box-Behnken designs</t>
+  </si>
+  <si>
+    <r>
+      <t>Box, G. E. P., &amp; Behnken, D. W. (1960). Simplex-sum designs: a class of second order rotatable designs derivable from those of first order.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> The Annals of Mathematical Statistics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 31(4), 838-864.</t>
+    </r>
+  </si>
+  <si>
+    <t>BBD_3F</t>
+  </si>
+  <si>
+    <t>BBD_4F</t>
+  </si>
+  <si>
+    <t>Uniform shell designs (Doehlert's designs)</t>
+  </si>
+  <si>
+    <r>
+      <t>Doehlert, D. H. (1970). Uniform shell designs.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> Journal of the Royal Statistical Society: Series C (Applied Statistics)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 19(3), 231-239.</t>
+    </r>
+  </si>
+  <si>
+    <t>DD_2F</t>
+  </si>
+  <si>
+    <t>DD_3F</t>
+  </si>
+  <si>
+    <t>DD_4F</t>
+  </si>
+  <si>
+    <t>Definitive screening designs</t>
+  </si>
+  <si>
+    <r>
+      <t>Jones, B., &amp; Nachtsheim, C. J. (2011). A class of three-level designs for definitive screening in the presence of second-order effects.</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> Journal of Quality Technology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 43(1), 1-15.</t>
+    </r>
+  </si>
+  <si>
+    <t>DSD</t>
+  </si>
 </sst>
 </file>
 
@@ -558,6 +751,17 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FFD4FF67"/>
+      <color rgb="FFDCC5ED"/>
+      <color rgb="FFBD92DE"/>
+      <color rgb="FF6DD9FF"/>
+      <color rgb="FFF69E9E"/>
+      <color rgb="FFFBBDF8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -869,7 +1073,7 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -879,24 +1083,24 @@
     <col min="15" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>64</v>
       </c>
@@ -916,7 +1120,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>65</v>
       </c>
@@ -939,7 +1143,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>83</v>
       </c>
@@ -956,7 +1160,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>67</v>
       </c>
@@ -967,7 +1171,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>89</v>
       </c>
@@ -976,7 +1180,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>88</v>
       </c>
@@ -990,93 +1194,151 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A14:N18"/>
+    <mergeCell ref="A19:N23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G6" location="'FF_2^3'!A1" display="'FF_2^3'!A1" xr:uid="{0E371BD0-6595-4F4D-95F3-87DA41F26BBF}"/>
@@ -1098,6 +1360,16 @@
     <hyperlink ref="I11" location="'L''36'!A1" display="'L''36'!A1" xr:uid="{4A186A22-2444-4C01-8768-875CC5AFBAA9}"/>
     <hyperlink ref="H8" location="'L27'!A1" display="'L27'!A1" xr:uid="{6D71B348-A68F-4382-809B-91E6FA1F1B3A}"/>
     <hyperlink ref="I8" location="'L9'!A1" display="'L9'!A1" xr:uid="{A1499175-FDDA-4175-9906-CF24E9538223}"/>
+    <hyperlink ref="G12" location="'YL8'!A1" display="'YL8'!A1" xr:uid="{74057CEB-606A-454B-8282-798F3780B29B}"/>
+    <hyperlink ref="G13" location="CCCD_2F!A1" display="CCCD_2F!A1" xr:uid="{0A2870D7-0C5F-4E0E-88E6-9478AC4ED75F}"/>
+    <hyperlink ref="H13" location="CCCD_3F!A1" display="CCCD_3F!A1" xr:uid="{428FC425-D9C1-45F3-959C-A8D1FB3CB5A4}"/>
+    <hyperlink ref="I13" location="CCCD_4F!A1" display="CCCD_4F!A1" xr:uid="{40FF4A5C-FF8A-42AC-A303-C16C1B614AF2}"/>
+    <hyperlink ref="G14" location="BBD_3F!A1" display="BBD_3F!A1" xr:uid="{261E4786-0C58-4149-B4DC-DBD4F570268F}"/>
+    <hyperlink ref="H14" location="BBD_4F!A1" display="BBD_4F" xr:uid="{F5006C7C-E9D5-4282-8999-F66C95805BE0}"/>
+    <hyperlink ref="G15" location="DD_2F!A1" display="DD_2F!A1" xr:uid="{0238097E-DE86-49BB-A4DA-E7780E479980}"/>
+    <hyperlink ref="H15" location="DD_3F!A1" display="DD_3F!A1" xr:uid="{296EC866-A699-4902-AEE6-A89B6C2358BF}"/>
+    <hyperlink ref="I15" location="DD_4F!A1" display="DD_4F!A1" xr:uid="{83735637-748F-4836-8319-7BA915D56D0A}"/>
+    <hyperlink ref="G16" location="DSD!A1" display="DSD!A1" xr:uid="{77D8FD32-1DD1-4FAC-9B0B-0F81642A0BB0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18911,6 +19183,3649 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11588A1A-5EFC-4E19-9BA4-32592583A529}">
+  <sheetPr>
+    <tabColor rgb="FFFBBDF8"/>
+  </sheetPr>
+  <dimension ref="A1:AJ13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="36" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>-1</v>
+      </c>
+      <c r="P2">
+        <v>-1</v>
+      </c>
+      <c r="Q2">
+        <v>-1</v>
+      </c>
+      <c r="R2">
+        <v>-1</v>
+      </c>
+      <c r="S2">
+        <v>-1</v>
+      </c>
+      <c r="T2">
+        <v>-1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>-1</v>
+      </c>
+      <c r="AH2">
+        <v>-1</v>
+      </c>
+      <c r="AI2">
+        <v>-1</v>
+      </c>
+      <c r="AJ2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+      <c r="H3">
+        <v>-1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>-1</v>
+      </c>
+      <c r="L3">
+        <v>-1</v>
+      </c>
+      <c r="M3">
+        <v>-1</v>
+      </c>
+      <c r="N3">
+        <v>-1</v>
+      </c>
+      <c r="O3">
+        <v>-1</v>
+      </c>
+      <c r="P3">
+        <v>-1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>-1</v>
+      </c>
+      <c r="AD3">
+        <v>-1</v>
+      </c>
+      <c r="AE3">
+        <v>-1</v>
+      </c>
+      <c r="AF3">
+        <v>-1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>-1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+      <c r="I4">
+        <v>-1</v>
+      </c>
+      <c r="J4">
+        <v>-1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>-1</v>
+      </c>
+      <c r="N4">
+        <v>-1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>-1</v>
+      </c>
+      <c r="R4">
+        <v>-1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>-1</v>
+      </c>
+      <c r="Z4">
+        <v>-1</v>
+      </c>
+      <c r="AA4">
+        <v>-1</v>
+      </c>
+      <c r="AB4">
+        <v>-1</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>-1</v>
+      </c>
+      <c r="J5">
+        <v>-1</v>
+      </c>
+      <c r="K5">
+        <v>-1</v>
+      </c>
+      <c r="L5">
+        <v>-1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>-1</v>
+      </c>
+      <c r="T5">
+        <v>-1</v>
+      </c>
+      <c r="U5">
+        <v>-1</v>
+      </c>
+      <c r="V5">
+        <v>-1</v>
+      </c>
+      <c r="W5">
+        <v>-1</v>
+      </c>
+      <c r="X5">
+        <v>-1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>-1</v>
+      </c>
+      <c r="G6">
+        <v>-1</v>
+      </c>
+      <c r="H6">
+        <v>-1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>-1</v>
+      </c>
+      <c r="V6">
+        <v>-1</v>
+      </c>
+      <c r="W6">
+        <v>-1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>-1</v>
+      </c>
+      <c r="Z6">
+        <v>-1</v>
+      </c>
+      <c r="AA6">
+        <v>-1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>-1</v>
+      </c>
+      <c r="AD6">
+        <v>-1</v>
+      </c>
+      <c r="AE6">
+        <v>-1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>-1</v>
+      </c>
+      <c r="AH6">
+        <v>-1</v>
+      </c>
+      <c r="AI6">
+        <v>-1</v>
+      </c>
+      <c r="AJ6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>-1</v>
+      </c>
+      <c r="J7">
+        <v>-1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>-1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>-1</v>
+      </c>
+      <c r="O7">
+        <v>-1</v>
+      </c>
+      <c r="P7">
+        <v>-1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>-1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>-1</v>
+      </c>
+      <c r="U7">
+        <v>-1</v>
+      </c>
+      <c r="V7">
+        <v>-1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>-1</v>
+      </c>
+      <c r="Y7">
+        <v>-1</v>
+      </c>
+      <c r="Z7">
+        <v>-1</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>-1</v>
+      </c>
+      <c r="AC7">
+        <v>-1</v>
+      </c>
+      <c r="AD7">
+        <v>-1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>-1</v>
+      </c>
+      <c r="AG7">
+        <v>-1</v>
+      </c>
+      <c r="AH7">
+        <v>-1</v>
+      </c>
+      <c r="AI7">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>-1</v>
+      </c>
+      <c r="K8">
+        <v>-1</v>
+      </c>
+      <c r="L8">
+        <v>-1</v>
+      </c>
+      <c r="M8">
+        <v>-1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>-1</v>
+      </c>
+      <c r="Q8">
+        <v>-1</v>
+      </c>
+      <c r="R8">
+        <v>-1</v>
+      </c>
+      <c r="S8">
+        <v>-1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>-1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>-1</v>
+      </c>
+      <c r="X8">
+        <v>-1</v>
+      </c>
+      <c r="Y8">
+        <v>-1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>-1</v>
+      </c>
+      <c r="AB8">
+        <v>-1</v>
+      </c>
+      <c r="AC8">
+        <v>-1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>-1</v>
+      </c>
+      <c r="AF8">
+        <v>-1</v>
+      </c>
+      <c r="AG8">
+        <v>-1</v>
+      </c>
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <v>-1</v>
+      </c>
+      <c r="AJ8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>-1</v>
+      </c>
+      <c r="I9">
+        <v>-1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>-1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>-1</v>
+      </c>
+      <c r="N9">
+        <v>-1</v>
+      </c>
+      <c r="O9">
+        <v>-1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>-1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>-1</v>
+      </c>
+      <c r="T9">
+        <v>-1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>-1</v>
+      </c>
+      <c r="W9">
+        <v>-1</v>
+      </c>
+      <c r="X9">
+        <v>-1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>-1</v>
+      </c>
+      <c r="AA9">
+        <v>-1</v>
+      </c>
+      <c r="AB9">
+        <v>-1</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AD9">
+        <v>-1</v>
+      </c>
+      <c r="AE9">
+        <v>-1</v>
+      </c>
+      <c r="AF9">
+        <v>-1</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>-1</v>
+      </c>
+      <c r="AI9">
+        <v>-1</v>
+      </c>
+      <c r="AJ9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:36" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="15" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B2:AT9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0821DBF-A7A9-44F7-9AD6-E7494E7006A7}">
+  <sheetPr>
+    <tabColor rgb="FF6DD9FF"/>
+  </sheetPr>
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1.4142135623730951</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>-1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:C14">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B720F53-383B-4D45-9B55-F6D6877FAAC4}">
+  <sheetPr>
+    <tabColor rgb="FF6DD9FF"/>
+  </sheetPr>
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-1.681792830507429</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1.681792830507429</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>-1.681792830507429</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1.681792830507429</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>-1.681792830507429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1.681792830507429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:D20">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78047FCB-3881-4731-BA1A-805049AD1DA9}">
+  <sheetPr>
+    <tabColor rgb="FF6DD9FF"/>
+  </sheetPr>
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>-1</v>
+      </c>
+      <c r="C14">
+        <v>-1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>-1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>-1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>-2</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>-2</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>-2</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:E31">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06919F78-C741-47B8-8508-8F4488D42E74}">
+  <sheetPr>
+    <tabColor rgb="FFDCC5ED"/>
+  </sheetPr>
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>-1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:D16">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2D66BA-DA45-46ED-A678-54DC41C54613}">
+  <sheetPr>
+    <tabColor rgb="FFDCC5ED"/>
+  </sheetPr>
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>-1</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>-1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>-1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>-1</v>
+      </c>
+      <c r="E22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>-1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:E28">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5288C6A8-0479-44E0-8F66-F0BC116719B5}">
+  <sheetPr>
+    <tabColor rgb="FFD4FF67"/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-0.5</v>
+      </c>
+      <c r="C5">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>-0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-0.5</v>
+      </c>
+      <c r="C7">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:C8">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E134BA-4169-41DE-80CF-978726153900}">
+  <sheetPr>
+    <tabColor rgb="FFD4FF67"/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-0.5</v>
+      </c>
+      <c r="C5">
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-0.5</v>
+      </c>
+      <c r="C7">
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-0.5</v>
+      </c>
+      <c r="C9">
+        <v>-0.28899999999999998</v>
+      </c>
+      <c r="D9">
+        <v>-0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>-0.28899999999999998</v>
+      </c>
+      <c r="D10">
+        <v>-0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-0.5</v>
+      </c>
+      <c r="C11">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="D11">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="D12">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>-0.57699999999999996</v>
+      </c>
+      <c r="D13">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="D14">
+        <v>-0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:D14">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D2D182-A71C-4718-8A7C-B13B7D8018D8}">
+  <sheetPr>
+    <tabColor rgb="FFD4FF67"/>
+  </sheetPr>
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-0.5</v>
+      </c>
+      <c r="C5">
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-0.5</v>
+      </c>
+      <c r="C7">
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-0.5</v>
+      </c>
+      <c r="C9">
+        <v>-0.28899999999999998</v>
+      </c>
+      <c r="D9">
+        <v>-0.81599999999999995</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="C10">
+        <v>-0.28899999999999998</v>
+      </c>
+      <c r="D10">
+        <v>-0.81599999999999995</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-0.5</v>
+      </c>
+      <c r="C11">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="D11">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="D12">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>-0.57699999999999996</v>
+      </c>
+      <c r="D13">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="D14">
+        <v>-0.81599999999999995</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>-0.5</v>
+      </c>
+      <c r="C15">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="D15">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.79100000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+      <c r="C16">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="D16">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.79100000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>-0.5</v>
+      </c>
+      <c r="C17">
+        <v>-0.28899999999999998</v>
+      </c>
+      <c r="D17">
+        <v>-0.20399999999999999</v>
+      </c>
+      <c r="E17">
+        <v>-0.79100000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+      <c r="C18">
+        <v>-0.28899999999999998</v>
+      </c>
+      <c r="D18">
+        <v>-0.20399999999999999</v>
+      </c>
+      <c r="E18">
+        <v>-0.79100000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>-0.57699999999999996</v>
+      </c>
+      <c r="D19">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.79100000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="D20">
+        <v>-0.20399999999999999</v>
+      </c>
+      <c r="E20">
+        <v>-0.79100000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>-0.61199999999999999</v>
+      </c>
+      <c r="E21">
+        <v>-0.79100000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="E22">
+        <v>-0.79100000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:E22">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8FE817-5C38-4E90-B35D-095E37386856}">
   <sheetPr>
@@ -19286,6 +23201,212 @@
   </sheetData>
   <conditionalFormatting sqref="B2:E17">
     <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC56C56-DAB7-48F1-B199-B1A269E1216E}">
+  <sheetPr>
+    <tabColor rgb="FFFF7C80"/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:E10">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Added additional DSD to CommonDesigns.xlsx
</commit_message>
<xml_diff>
--- a/CommonDesigns.xlsx
+++ b/CommonDesigns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jordi_Classes_234\DOE\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4DBF89-49E5-4B54-9119-E64E5E881BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9155BB2-F8FB-4054-A7EE-4E736699DAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B1F4CC8-6E29-4DF5-9B9B-812FEB45778E}"/>
   </bookViews>
@@ -42,7 +42,10 @@
     <sheet name="DD_2F" sheetId="32" r:id="rId27"/>
     <sheet name="DD_3F" sheetId="31" r:id="rId28"/>
     <sheet name="DD_4F" sheetId="30" r:id="rId29"/>
-    <sheet name="DSD" sheetId="33" r:id="rId30"/>
+    <sheet name="DSD9" sheetId="33" r:id="rId30"/>
+    <sheet name="DSD11" sheetId="36" r:id="rId31"/>
+    <sheet name="DSD13" sheetId="34" r:id="rId32"/>
+    <sheet name="DSD15" sheetId="35" r:id="rId33"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="126">
   <si>
     <t>A</t>
   </si>
@@ -656,7 +659,22 @@
     </r>
   </si>
   <si>
-    <t>DSD</t>
+    <t>This design can be used for a reduced number of factors</t>
+  </si>
+  <si>
+    <t>by droping the last columns</t>
+  </si>
+  <si>
+    <t>DSD9</t>
+  </si>
+  <si>
+    <t>DSD11</t>
+  </si>
+  <si>
+    <t>DSD13</t>
+  </si>
+  <si>
+    <t>DSD15</t>
   </si>
 </sst>
 </file>
@@ -1248,8 +1266,17 @@
       <c r="B16" t="s">
         <v>118</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>120</v>
+      <c r="G16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1396,10 @@
     <hyperlink ref="G15" location="DD_2F!A1" display="DD_2F!A1" xr:uid="{0238097E-DE86-49BB-A4DA-E7780E479980}"/>
     <hyperlink ref="H15" location="DD_3F!A1" display="DD_3F!A1" xr:uid="{296EC866-A699-4902-AEE6-A89B6C2358BF}"/>
     <hyperlink ref="I15" location="DD_4F!A1" display="DD_4F!A1" xr:uid="{83735637-748F-4836-8319-7BA915D56D0A}"/>
-    <hyperlink ref="G16" location="DSD!A1" display="DSD!A1" xr:uid="{77D8FD32-1DD1-4FAC-9B0B-0F81642A0BB0}"/>
+    <hyperlink ref="G16" location="'DSD9'!A1" display="'DSD9'!A1" xr:uid="{EAAA1907-059F-460E-9766-46A0ECCAD8B2}"/>
+    <hyperlink ref="H16" location="'DSD11'!A1" display="'DSD11'!A1" xr:uid="{98A87E70-09E5-43DC-804D-52D1DDA8FB5F}"/>
+    <hyperlink ref="I16" location="'DSD13'!A1" display="'DSD13'!A1" xr:uid="{17E54BFA-D1F2-447C-BB9F-E40D03FD367F}"/>
+    <hyperlink ref="J16" location="'DSD15'!A1" display="'DSD15'!A1" xr:uid="{27AB891E-2F3A-4765-97DE-6F3D39A0CB7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23407,6 +23437,1110 @@
   </sheetData>
   <conditionalFormatting sqref="B2:E10">
     <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6D7104-044F-4591-9B22-DB13C9E64AAD}">
+  <sheetPr>
+    <tabColor rgb="FFFF7C80"/>
+  </sheetPr>
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-1</v>
+      </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:F12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D6DAE5-43DB-4A9D-BF43-1FB5EE6FD6A6}">
+  <sheetPr>
+    <tabColor rgb="FFFF7C80"/>
+  </sheetPr>
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="7" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>-1</v>
+      </c>
+      <c r="G6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>-1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>-1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>-1</v>
+      </c>
+      <c r="C13">
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:G14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.39997558519241921"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="4" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F095E8-9D39-4598-8792-5F82BAF1B18A}">
+  <sheetPr>
+    <tabColor rgb="FFFF7C80"/>
+  </sheetPr>
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="8" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>-1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>-1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>-1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <v>-1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>-1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>-1</v>
+      </c>
+      <c r="C15">
+        <v>-1</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+      <c r="E15">
+        <v>-1</v>
+      </c>
+      <c r="F15">
+        <v>-1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="B2:H16">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>